<commit_message>
Added Spanish and formal German language support.
</commit_message>
<xml_diff>
--- a/data-raw/JAJ_dict.xlsx
+++ b/data-raw/JAJ_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\JAJ\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38D53DB-8744-49EE-A998-FD62D2BAD44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC4CF05-25B0-42BB-8692-736FAF45B69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="289">
   <si>
     <t>key</t>
   </si>
@@ -674,6 +674,219 @@
   </si>
   <si>
     <t>E poichè dopo è andata qui, allora clicca qui.</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Bienvenido/a al Test de Memoria de Trabajo de Jack y Jill</t>
+  </si>
+  <si>
+    <t>Jack gira cada vez que contestarás a esta pregunta: “¿Jack tiene la bolita en la misma mano que Jill?”Antes de responder, memoriza dónde está la bolita.</t>
+  </si>
+  <si>
+    <t>Continuar</t>
+  </si>
+  <si>
+    <t>Haz clic en los circulitos naranjas donde viste la bolita desplazarse en el mismo orden en el que Jack giró.</t>
+  </si>
+  <si>
+    <t>Has terminado el Test de Memoria de Jack y Jill.</t>
+  </si>
+  <si>
+    <t>Pregunta {{num_question}} de {{test_length}}</t>
+  </si>
+  <si>
+    <t>Por favor inserta solo dígitos sin espacios</t>
+  </si>
+  <si>
+    <t>Ejemplo {{num_example}}</t>
+  </si>
+  <si>
+    <t>Tu acceso no es válido. Por favor, inténtalo de nuevo.</t>
+  </si>
+  <si>
+    <t>Te recordaste el {{prop_correct_hand}}% de manos y el {{prop_correct_position}}% de secuencias correctamente.</t>
+  </si>
+  <si>
+    <t>Tenías razón sobre en qué mano Jack tenía la bolita.</t>
+  </si>
+  <si>
+    <t>No tenías razón sobre en qué mano Jack tenía la bolita.</t>
+  </si>
+  <si>
+    <t>Ahora vamos a empezar la prueba principal en la cual no recibirás ninguna retroalimentación. ¡Disfruta!</t>
+  </si>
+  <si>
+    <t>Por favor, inserta tu código de participante</t>
+  </si>
+  <si>
+    <t>ej. 10492817</t>
+  </si>
+  <si>
+    <t>Por favor inserta un código valido.</t>
+  </si>
+  <si>
+    <t>Tenías razón sobre el orden en el cual se desplazó la bolita.</t>
+  </si>
+  <si>
+    <t>No tenías razón sobre el orden en el cual se desplazó la bolita.</t>
+  </si>
+  <si>
+    <t>Misma</t>
+  </si>
+  <si>
+    <t>Distinta</t>
+  </si>
+  <si>
+    <t>Está Jill a la izquierda y Jack a la derecha de la pantalla. Cada uno de ellos tiene una bolita azul en la mano.</t>
+  </si>
+  <si>
+    <t>¿Jack tiene la bolita en la misma mano que Jill? Recuerda dónde está la bolita cuando Jack gira.</t>
+  </si>
+  <si>
+    <t>¡Hagamos un poco de práctica!</t>
+  </si>
+  <si>
+    <t>Haz clic en el circulito naranja donde viste la bolita desplazarse en el mismo orden en el que Jack giró.</t>
+  </si>
+  <si>
+    <t>Ingresa tu dirección de correo electrónico a continuación para tu compensación de **Slicethepie**.</t>
+  </si>
+  <si>
+    <t>Tu correo electrónico</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>¡Gracias por participar!</t>
+  </si>
+  <si>
+    <t>Ahora puedes cerrar la ventana de tu navegador.</t>
+  </si>
+  <si>
+    <t>Tus resultados han sido guardados.</t>
+  </si>
+  <si>
+    <t>Ahora haz clic en el circulito que estaba cubierto por la bolita.</t>
+  </si>
+  <si>
+    <t>**Enhorabuena**!\\Para pasar cada ronda tendrás que: 1) saber si Jack y Jill tienen la bolita en la misma mano, 2) recordar dónde va la bolita cada vez que Jack gira.</t>
+  </si>
+  <si>
+    <t>Detrás de Jack hay 6 circulitos naranjas. Jill no se mueve, pero Jack puede girar, como puedes ver aquí. Cuando Jack gira, la bolita en su mano cubre uno de los circulitos detrás de él. **En cada ronda, recuerda qué circulo se cubre con la bola.**</t>
+  </si>
+  <si>
+    <t>Jack también puede girar más de una vez en la misma ronda. Ahora Jack tiene la bolita en la misma mano que Jill. Haz clic en “Misma”. Recuerda el circulito cubierto por la bolita.</t>
+  </si>
+  <si>
+    <t>Y ahora para la segunda ronda, Jack tiene la bolita en una mano distinta. Haz clic en “Distinta”. Recuerda el circulito cubierto por la bolita.</t>
+  </si>
+  <si>
+    <t>Ahora haz clic en los dos sitios a los que se desplazó la bolita cuando Jack giró, en el mismo orden. Como la bolita se desplazó aquí primero, entonces haz clic aquí.</t>
+  </si>
+  <si>
+    <t>Y como luego se desplazó aquí, entonces haz clic aquí.</t>
+  </si>
+  <si>
+    <t>Ahora intenta tú solo/a sin ayuda.</t>
+  </si>
+  <si>
+    <t>Test de Memoria de Jack y Jill</t>
+  </si>
+  <si>
+    <t>Contestaste {{num_correct}} de {{num_question}} secuencias de posición correctamente.</t>
+  </si>
+  <si>
+    <t>Tu puntuación</t>
+  </si>
+  <si>
+    <t>Puntuación</t>
+  </si>
+  <si>
+    <t>DE_F</t>
+  </si>
+  <si>
+    <t>Johann dreht sich jedesmal, nachdem Sie die folgende Frage beantwortet haben: „Hatte Johann den Ball in der gleichen Hand wie Johanna?" Bevor sie antworten, merke Sie sich bitte, auf welcher Position der Ball war.</t>
+  </si>
+  <si>
+    <t>Bitte klicken Sie auf die Positionen der Bälle in der Reihenfolge, die Sie gesehen hast.</t>
+  </si>
+  <si>
+    <t>Sie haben den Johann &amp; Johanna Gedächtnistest beendet.</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie nur Ziffern ohne Leerzeichen ein.</t>
+  </si>
+  <si>
+    <t>Ihre Eingabe war nicht korrekt. Bitte versuchen Sie noch mal.</t>
+  </si>
+  <si>
+    <t>Sie hatten {{prop_correct_hand}}% der Ballhände und {{prop_correct_position}}% der Ballpositionen richtig.</t>
+  </si>
+  <si>
+    <t>Jetzt geht es weiter zum Haupttest, in dem Sie keine Rückmeldung mehr bekommen. Viel Spaß!</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie Ihre ID ein</t>
+  </si>
+  <si>
+    <t>Johanna hält den Ball immer rechts (**von Ihnen  aus gesehen**), aber Johann kann ihn links oder rechts halten. Hier hat er ihn links, also nicht in der gleichen Hand wie Johanna.  Klicken Sie auf „Verschieden" und merken Sie sich die Ballposition.</t>
+  </si>
+  <si>
+    <t>Hält Johann den Ball in der gleichen Hand wie Johanna? Merke Sie sich bitte, wo der Ball ist, wenn Johann sich dreht.</t>
+  </si>
+  <si>
+    <t>Sie können das nun ausprobieren.</t>
+  </si>
+  <si>
+    <t>Klicken Sie die Positionen von Johanns Ball in der richtigen Reihenfolge.</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie ihre E-Mail-Adresse für ihre Slicethepie Kompensation ein.</t>
+  </si>
+  <si>
+    <t>Ihre Email-Adresse</t>
+  </si>
+  <si>
+    <t>Danke für Ihre Teilnahme!</t>
+  </si>
+  <si>
+    <t>Sie können den Browsertab jetzt schließen.</t>
+  </si>
+  <si>
+    <t>Ihre Ergebnisse wurden gespeichert.</t>
+  </si>
+  <si>
+    <t>Jetzt klicken Sie bitte auf die Position, wo der Ball war.</t>
+  </si>
+  <si>
+    <t>Hinter Johann sind 6 verschiedene orangene Punkte. Johanna kann sich nicht bewegen, aber Johann kann sich drehen. Wenn Johann sich dreht, wird sein Ball einen der Punkte hinter ihm verdecken. **Merke Sie sich bitte bei jeder Drehung, auf welchem Punkt der Ball war.**</t>
+  </si>
+  <si>
+    <t>Das Ganze geht auch mit mehr als einer Drehung. Hier hat Johann den Ball in der gleichen Hand. Klicken Sie unten auf „Gleich" und merken Sie sich, wo der Ball war.</t>
+  </si>
+  <si>
+    <t>Bei der nächsten Drehung hat Johann den Ball in der anderen Hand. Klicken Sie also unten auf „Verschieden". Merken Sie sich immer, wo der Ball war.</t>
+  </si>
+  <si>
+    <t>Zuerst war der Ball hier beim roten Pfeil, bitte klicken Sie darauf.</t>
+  </si>
+  <si>
+    <t>Dann war er hier. Also klicken Sie auf den Punkt beim rotem Pfeil.</t>
+  </si>
+  <si>
+    <t>Nun versuchen Sie selbst ohne Hilfe.</t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} von {{num_question}} Ballfolgen richtig beantwortet.</t>
+  </si>
+  <si>
+    <t>Ihr Testergebnis</t>
+  </si>
+  <si>
+    <t>Jill siempre tendrá la bolita en su mano derecha **desde tu punto de vista**, pero jack puede tener la bolita en su mano izquierda o derecha.\\ Aquí la tiene en la mano izquierda, distinta de la de Jill. Haz clic en “distinta” abajo y recuerda también el circulito que la bolita cubre.</t>
   </si>
 </sst>
 </file>
@@ -1517,18 +1730,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="81.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="81.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1536,16 +1749,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1553,16 +1772,22 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1570,16 +1795,22 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1587,16 +1818,22 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1604,16 +1841,22 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1621,16 +1864,22 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1638,16 +1887,22 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1655,16 +1910,22 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1672,16 +1933,22 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1689,16 +1956,22 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1706,16 +1979,22 @@
         <v>41</v>
       </c>
       <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1723,16 +2002,22 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1740,16 +2025,22 @@
         <v>49</v>
       </c>
       <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1757,16 +2048,22 @@
         <v>53</v>
       </c>
       <c r="C14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1774,16 +2071,22 @@
         <v>57</v>
       </c>
       <c r="C15" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1791,16 +2094,22 @@
         <v>61</v>
       </c>
       <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1808,16 +2117,22 @@
         <v>65</v>
       </c>
       <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1825,16 +2140,22 @@
         <v>69</v>
       </c>
       <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1842,16 +2163,22 @@
         <v>73</v>
       </c>
       <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -1859,16 +2186,22 @@
         <v>77</v>
       </c>
       <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
         <v>78</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1876,16 +2209,22 @@
         <v>81</v>
       </c>
       <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1893,16 +2232,22 @@
         <v>85</v>
       </c>
       <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
         <v>86</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1910,16 +2255,22 @@
         <v>89</v>
       </c>
       <c r="C23" t="s">
+        <v>270</v>
+      </c>
+      <c r="D23" t="s">
         <v>90</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -1927,16 +2278,22 @@
         <v>93</v>
       </c>
       <c r="C24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D24" t="s">
         <v>94</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -1944,16 +2301,22 @@
         <v>97</v>
       </c>
       <c r="C25" t="s">
+        <v>272</v>
+      </c>
+      <c r="D25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -1961,16 +2324,22 @@
         <v>101</v>
       </c>
       <c r="C26" t="s">
+        <v>273</v>
+      </c>
+      <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -1978,16 +2347,22 @@
         <v>103</v>
       </c>
       <c r="C27" t="s">
+        <v>274</v>
+      </c>
+      <c r="D27" t="s">
         <v>104</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -1995,16 +2370,22 @@
         <v>107</v>
       </c>
       <c r="C28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D28" t="s">
         <v>108</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -2012,16 +2393,22 @@
         <v>111</v>
       </c>
       <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
         <v>112</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -2029,16 +2416,22 @@
         <v>115</v>
       </c>
       <c r="C30" t="s">
+        <v>276</v>
+      </c>
+      <c r="D30" t="s">
         <v>116</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -2046,16 +2439,22 @@
         <v>119</v>
       </c>
       <c r="C31" t="s">
+        <v>277</v>
+      </c>
+      <c r="D31" t="s">
         <v>120</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>122</v>
       </c>
@@ -2063,16 +2462,22 @@
         <v>123</v>
       </c>
       <c r="C32" t="s">
+        <v>278</v>
+      </c>
+      <c r="D32" t="s">
         <v>124</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -2080,16 +2485,22 @@
         <v>127</v>
       </c>
       <c r="C33" t="s">
+        <v>279</v>
+      </c>
+      <c r="D33" t="s">
         <v>128</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G33" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -2097,16 +2508,22 @@
         <v>131</v>
       </c>
       <c r="C34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" t="s">
         <v>132</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>133</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="G34" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -2114,16 +2531,22 @@
         <v>135</v>
       </c>
       <c r="C35" t="s">
+        <v>280</v>
+      </c>
+      <c r="D35" t="s">
         <v>136</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>137</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G35" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -2131,16 +2554,22 @@
         <v>139</v>
       </c>
       <c r="C36" t="s">
+        <v>281</v>
+      </c>
+      <c r="D36" t="s">
         <v>140</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>141</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G36" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -2148,16 +2577,22 @@
         <v>143</v>
       </c>
       <c r="C37" t="s">
+        <v>282</v>
+      </c>
+      <c r="D37" t="s">
         <v>144</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>146</v>
       </c>
@@ -2165,16 +2600,22 @@
         <v>147</v>
       </c>
       <c r="C38" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" t="s">
         <v>148</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -2182,16 +2623,22 @@
         <v>151</v>
       </c>
       <c r="C39" t="s">
+        <v>284</v>
+      </c>
+      <c r="D39" t="s">
         <v>152</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>153</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G39" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -2199,16 +2646,22 @@
         <v>131</v>
       </c>
       <c r="C40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" t="s">
         <v>155</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>133</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>156</v>
       </c>
@@ -2216,16 +2669,22 @@
         <v>157</v>
       </c>
       <c r="C41" t="s">
+        <v>285</v>
+      </c>
+      <c r="D41" t="s">
         <v>158</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>159</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>160</v>
       </c>
@@ -2233,16 +2692,22 @@
         <v>161</v>
       </c>
       <c r="C42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" t="s">
         <v>162</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -2250,16 +2715,22 @@
         <v>165</v>
       </c>
       <c r="C43" t="s">
+        <v>286</v>
+      </c>
+      <c r="D43" t="s">
         <v>166</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>167</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>168</v>
       </c>
@@ -2267,16 +2738,22 @@
         <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>170</v>
+        <v>287</v>
       </c>
       <c r="D44" t="s">
         <v>170</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>171</v>
       </c>
@@ -2284,13 +2761,19 @@
         <v>172</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D45" t="s">
         <v>173</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
+        <v>173</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>205</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>